<commit_message>
Updated Instant Meeting test case
</commit_message>
<xml_diff>
--- a/TestData/TestDataFile.xlsx
+++ b/TestData/TestDataFile.xlsx
@@ -228,7 +228,7 @@
     <t>https://meet2.synesisit.info/m/j/647712840966/kakonpaulavi</t>
   </si>
   <si>
-    <t>https://meet2.synesisit.info/m/j/418121303608/mosharof?pwd=ddd8f1777358c471f7858faf00f71b89</t>
+    <t>https://meet2.synesisit.info/m/j/418121303608/mosharof</t>
   </si>
 </sst>
 </file>
@@ -1069,12 +1069,12 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="86.36328125" style="8" customWidth="1"/>
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="52.36328125" style="8" customWidth="1"/>
     <col min="2" max="16384" width="8.7265625" style="8"/>
   </cols>
   <sheetData>
@@ -1096,7 +1096,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" display="https://meet2.synesisit.info/m/j/418121303608/mosharof?pwd=ddd8f1777358c471f7858faf00f71b88"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://meet2.synesisit.info/m/j/418121303608/mosharof?pwd=ddd8f1777358c471f7858faf00f71b88"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Convay Middle Layer Automation
</commit_message>
<xml_diff>
--- a/TestData/TestDataFile.xlsx
+++ b/TestData/TestDataFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" tabRatio="868" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" tabRatio="868" firstSheet="12" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Login-Credential" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
   <si>
     <t>UserThree</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Invitation</t>
   </si>
   <si>
-    <t>test841@gmail.com</t>
-  </si>
-  <si>
     <t>UpdatedPMU</t>
   </si>
   <si>
@@ -207,15 +204,6 @@
     <t>No Reason</t>
   </si>
   <si>
-    <t>doyohi7376@paxnw.com</t>
-  </si>
-  <si>
-    <t>fiyel82061@adambra.com</t>
-  </si>
-  <si>
-    <t>miledeh490@digopm.com</t>
-  </si>
-  <si>
     <t>Edited</t>
   </si>
   <si>
@@ -225,10 +213,28 @@
     <t>https://meet2.synesisit.info/m/j/647712840966/kakonpaulavi</t>
   </si>
   <si>
-    <t>https://meet2.synesisit.info/m/j/418121303608/mosharof</t>
-  </si>
-  <si>
-    <t>bilaha2222@lieboe.com</t>
+    <t>loxowik819@daxiake.com</t>
+  </si>
+  <si>
+    <t>test8877@gmail.com</t>
+  </si>
+  <si>
+    <t>rinag46116@coderdir.com</t>
+  </si>
+  <si>
+    <t>https://meet2.synesisit.info/m/j/418121303608/mhsujan</t>
+  </si>
+  <si>
+    <t>dasedem563@makroyal.com</t>
+  </si>
+  <si>
+    <t>Abcd1234+</t>
+  </si>
+  <si>
+    <t>jinobic767@jxbav.com</t>
+  </si>
+  <si>
+    <t>Abcd12345+</t>
   </si>
 </sst>
 </file>
@@ -606,7 +612,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -661,7 +667,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -690,7 +696,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -716,10 +722,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
         <v>46</v>
-      </c>
-      <c r="B1" t="s">
-        <v>47</v>
       </c>
       <c r="C1" s="3">
         <v>1215</v>
@@ -748,10 +754,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -779,19 +785,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
         <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -807,8 +813,8 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -819,15 +825,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -844,9 +850,7 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -856,7 +860,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -877,45 +881,46 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
     <col min="2" max="2" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>40</v>
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="miledeh490@digopm.com"/>
-    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -935,7 +940,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
@@ -955,7 +960,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -970,15 +975,15 @@
         <v>647712840966</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -986,7 +991,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1019,7 +1024,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1036,8 +1041,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1052,15 +1057,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1069,7 +1071,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1085,7 +1087,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
@@ -1159,7 +1161,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1200,7 +1202,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
         <v>30</v>
@@ -1297,7 +1299,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1325,7 +1327,7 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3">
         <v>1724877700</v>
@@ -1340,10 +1342,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1356,7 +1358,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -1365,21 +1367,21 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
         <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1387,19 +1389,21 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="B3:C3" r:id="rId1" display="Pk125058@"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1411,7 +1415,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1423,7 +1427,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1431,10 +1435,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor Changes 4th Sept
</commit_message>
<xml_diff>
--- a/TestData/TestDataFile.xlsx
+++ b/TestData/TestDataFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" tabRatio="868" firstSheet="12" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" tabRatio="868" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login-Credential" sheetId="1" r:id="rId1"/>
@@ -213,9 +213,6 @@
     <t>https://meet2.synesisit.info/m/j/647712840966/kakonpaulavi</t>
   </si>
   <si>
-    <t>loxowik819@daxiake.com</t>
-  </si>
-  <si>
     <t>test8877@gmail.com</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t>Abcd12345+</t>
+  </si>
+  <si>
+    <t>loxowik130@daxiake.com</t>
   </si>
 </sst>
 </file>
@@ -813,7 +813,7 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -830,10 +830,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
         <v>60</v>
-      </c>
-      <c r="B2" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -860,7 +860,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -892,26 +892,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
         <v>62</v>
-      </c>
-      <c r="B3" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1041,8 +1041,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1057,12 +1057,15 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1087,7 +1090,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
@@ -1202,7 +1205,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
         <v>30</v>

</xml_diff>